<commit_message>
export ob and to
</commit_message>
<xml_diff>
--- a/library/to_export_date.xlsx
+++ b/library/to_export_date.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\fas\library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{952BFC1C-FD91-4FDE-9393-6075A739D2CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0157EE7D-B475-4C21-9830-3E93693F7E5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="23055" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="22980" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$J$58</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$J$31</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -82,10 +82,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
     <numFmt numFmtId="165" formatCode="mm&quot;/&quot;dd&quot;/&quot;yyyy"/>
-    <numFmt numFmtId="166" formatCode="m/d/yyyy"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -173,7 +172,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -217,19 +216,6 @@
         <color rgb="FF000000"/>
       </right>
       <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
@@ -287,7 +273,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -346,48 +332,6 @@
     <xf numFmtId="165" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="18" fontId="8" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="18" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="18" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -395,21 +339,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -433,16 +362,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -762,10 +691,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J938"/>
+  <dimension ref="A1:J911"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A16" zoomScale="60" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="37.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -809,24 +738,24 @@
         <v>0</v>
       </c>
       <c r="B3" s="1"/>
-      <c r="D3" s="44" t="s">
+      <c r="D3" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="44"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
       <c r="I3" s="7"/>
     </row>
     <row r="4" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2"/>
-      <c r="D4" s="44" t="s">
+      <c r="D4" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="44"/>
-      <c r="F4" s="44"/>
-      <c r="G4" s="44"/>
-      <c r="H4" s="44"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
       <c r="I4" s="7"/>
     </row>
     <row r="5" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -841,55 +770,55 @@
       <c r="I5" s="8"/>
     </row>
     <row r="6" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="47" t="s">
+      <c r="A6" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="47" t="s">
+      <c r="B6" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="49" t="s">
+      <c r="C6" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="52" t="s">
+      <c r="D6" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="52"/>
-      <c r="F6" s="50" t="s">
+      <c r="E6" s="33"/>
+      <c r="F6" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="45" t="s">
+      <c r="G6" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="45" t="s">
+      <c r="H6" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="I6" s="45" t="s">
+      <c r="I6" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="J6" s="42" t="s">
+      <c r="J6" s="23" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="48"/>
-      <c r="B7" s="48"/>
-      <c r="C7" s="46"/>
+      <c r="A7" s="29"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="27"/>
       <c r="D7" s="9" t="s">
         <v>3</v>
       </c>
       <c r="E7" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="51"/>
-      <c r="G7" s="46"/>
-      <c r="H7" s="46"/>
-      <c r="I7" s="46"/>
-      <c r="J7" s="43"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="27"/>
+      <c r="J7" s="24"/>
     </row>
     <row r="8" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13"/>
       <c r="B8" s="14"/>
-      <c r="C8" s="34"/>
+      <c r="C8" s="20"/>
       <c r="D8" s="15"/>
       <c r="E8" s="16"/>
       <c r="F8" s="16"/>
@@ -901,7 +830,7 @@
     <row r="9" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13"/>
       <c r="B9" s="14"/>
-      <c r="C9" s="34"/>
+      <c r="C9" s="20"/>
       <c r="D9" s="15"/>
       <c r="E9" s="16"/>
       <c r="F9" s="16"/>
@@ -913,7 +842,7 @@
     <row r="10" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13"/>
       <c r="B10" s="14"/>
-      <c r="C10" s="34"/>
+      <c r="C10" s="20"/>
       <c r="D10" s="15"/>
       <c r="E10" s="16"/>
       <c r="F10" s="16"/>
@@ -925,7 +854,7 @@
     <row r="11" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="13"/>
       <c r="B11" s="14"/>
-      <c r="C11" s="34"/>
+      <c r="C11" s="20"/>
       <c r="D11" s="15"/>
       <c r="E11" s="16"/>
       <c r="F11" s="16"/>
@@ -937,7 +866,7 @@
     <row r="12" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="13"/>
       <c r="B12" s="14"/>
-      <c r="C12" s="34"/>
+      <c r="C12" s="20"/>
       <c r="D12" s="15"/>
       <c r="E12" s="15"/>
       <c r="F12" s="15"/>
@@ -949,7 +878,7 @@
     <row r="13" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="13"/>
       <c r="B13" s="14"/>
-      <c r="C13" s="34"/>
+      <c r="C13" s="20"/>
       <c r="D13" s="15"/>
       <c r="E13" s="16"/>
       <c r="F13" s="16"/>
@@ -961,7 +890,7 @@
     <row r="14" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13"/>
       <c r="B14" s="14"/>
-      <c r="C14" s="34"/>
+      <c r="C14" s="20"/>
       <c r="D14" s="15"/>
       <c r="E14" s="16"/>
       <c r="F14" s="16"/>
@@ -973,7 +902,7 @@
     <row r="15" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="13"/>
       <c r="B15" s="16"/>
-      <c r="C15" s="34"/>
+      <c r="C15" s="20"/>
       <c r="D15" s="15"/>
       <c r="E15" s="15"/>
       <c r="F15" s="15"/>
@@ -985,7 +914,7 @@
     <row r="16" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="13"/>
       <c r="B16" s="16"/>
-      <c r="C16" s="34"/>
+      <c r="C16" s="20"/>
       <c r="D16" s="15"/>
       <c r="E16" s="16"/>
       <c r="F16" s="16"/>
@@ -997,7 +926,7 @@
     <row r="17" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="13"/>
       <c r="B17" s="14"/>
-      <c r="C17" s="35"/>
+      <c r="C17" s="21"/>
       <c r="D17" s="15"/>
       <c r="E17" s="16"/>
       <c r="F17" s="16"/>
@@ -1009,7 +938,7 @@
     <row r="18" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="13"/>
       <c r="B18" s="19"/>
-      <c r="C18" s="36"/>
+      <c r="C18" s="22"/>
       <c r="D18" s="15"/>
       <c r="E18" s="16"/>
       <c r="F18" s="16"/>
@@ -1021,7 +950,7 @@
     <row r="19" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="13"/>
       <c r="B19" s="14"/>
-      <c r="C19" s="36"/>
+      <c r="C19" s="22"/>
       <c r="D19" s="15"/>
       <c r="E19" s="16"/>
       <c r="F19" s="16"/>
@@ -1033,7 +962,7 @@
     <row r="20" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="13"/>
       <c r="B20" s="14"/>
-      <c r="C20" s="34"/>
+      <c r="C20" s="20"/>
       <c r="D20" s="15"/>
       <c r="E20" s="16"/>
       <c r="F20" s="16"/>
@@ -1045,7 +974,7 @@
     <row r="21" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="13"/>
       <c r="B21" s="14"/>
-      <c r="C21" s="34"/>
+      <c r="C21" s="20"/>
       <c r="D21" s="15"/>
       <c r="E21" s="16"/>
       <c r="F21" s="16"/>
@@ -1057,7 +986,7 @@
     <row r="22" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="13"/>
       <c r="B22" s="14"/>
-      <c r="C22" s="34"/>
+      <c r="C22" s="20"/>
       <c r="D22" s="16"/>
       <c r="E22" s="16"/>
       <c r="F22" s="16"/>
@@ -1069,7 +998,7 @@
     <row r="23" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="13"/>
       <c r="B23" s="14"/>
-      <c r="C23" s="34"/>
+      <c r="C23" s="20"/>
       <c r="D23" s="15"/>
       <c r="E23" s="16"/>
       <c r="F23" s="16"/>
@@ -1081,7 +1010,7 @@
     <row r="24" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="13"/>
       <c r="B24" s="14"/>
-      <c r="C24" s="34"/>
+      <c r="C24" s="20"/>
       <c r="D24" s="16"/>
       <c r="E24" s="16"/>
       <c r="F24" s="16"/>
@@ -1093,7 +1022,7 @@
     <row r="25" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="13"/>
       <c r="B25" s="14"/>
-      <c r="C25" s="34"/>
+      <c r="C25" s="20"/>
       <c r="D25" s="15"/>
       <c r="E25" s="16"/>
       <c r="F25" s="16"/>
@@ -1105,7 +1034,7 @@
     <row r="26" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="13"/>
       <c r="B26" s="14"/>
-      <c r="C26" s="34"/>
+      <c r="C26" s="20"/>
       <c r="D26" s="15"/>
       <c r="E26" s="16"/>
       <c r="F26" s="16"/>
@@ -1117,7 +1046,7 @@
     <row r="27" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="13"/>
       <c r="B27" s="14"/>
-      <c r="C27" s="34"/>
+      <c r="C27" s="20"/>
       <c r="D27" s="15"/>
       <c r="E27" s="16"/>
       <c r="F27" s="16"/>
@@ -1129,7 +1058,7 @@
     <row r="28" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="13"/>
       <c r="B28" s="14"/>
-      <c r="C28" s="34"/>
+      <c r="C28" s="20"/>
       <c r="D28" s="15"/>
       <c r="E28" s="16"/>
       <c r="F28" s="16"/>
@@ -1141,7 +1070,7 @@
     <row r="29" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="13"/>
       <c r="B29" s="14"/>
-      <c r="C29" s="34"/>
+      <c r="C29" s="20"/>
       <c r="D29" s="15"/>
       <c r="E29" s="15"/>
       <c r="F29" s="15"/>
@@ -1153,7 +1082,7 @@
     <row r="30" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="13"/>
       <c r="B30" s="14"/>
-      <c r="C30" s="34"/>
+      <c r="C30" s="20"/>
       <c r="D30" s="15"/>
       <c r="E30" s="15"/>
       <c r="F30" s="15"/>
@@ -1165,7 +1094,7 @@
     <row r="31" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="13"/>
       <c r="B31" s="14"/>
-      <c r="C31" s="34"/>
+      <c r="C31" s="20"/>
       <c r="D31" s="15"/>
       <c r="E31" s="15"/>
       <c r="F31" s="15"/>
@@ -1175,330 +1104,303 @@
       <c r="J31" s="18"/>
     </row>
     <row r="32" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="13"/>
-      <c r="B32" s="14"/>
-      <c r="C32" s="34"/>
-      <c r="D32" s="15"/>
-      <c r="E32" s="15"/>
-      <c r="F32" s="15"/>
-      <c r="G32" s="17"/>
-      <c r="H32" s="17"/>
-      <c r="I32" s="17"/>
-      <c r="J32" s="18"/>
-    </row>
-    <row r="33" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="13"/>
-      <c r="B33" s="14"/>
-      <c r="C33" s="34"/>
-      <c r="D33" s="15"/>
-      <c r="E33" s="15"/>
-      <c r="F33" s="15"/>
-      <c r="G33" s="17"/>
-      <c r="H33" s="17"/>
-      <c r="I33" s="17"/>
-      <c r="J33" s="18"/>
-    </row>
-    <row r="34" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="13"/>
-      <c r="B34" s="14"/>
-      <c r="C34" s="34"/>
-      <c r="D34" s="15"/>
-      <c r="E34" s="15"/>
-      <c r="F34" s="15"/>
-      <c r="G34" s="17"/>
-      <c r="H34" s="17"/>
-      <c r="I34" s="17"/>
-      <c r="J34" s="18"/>
-    </row>
-    <row r="35" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="13"/>
-      <c r="B35" s="14"/>
-      <c r="C35" s="34"/>
-      <c r="D35" s="15"/>
-      <c r="E35" s="15"/>
-      <c r="F35" s="15"/>
-      <c r="G35" s="17"/>
-      <c r="H35" s="17"/>
-      <c r="I35" s="17"/>
-      <c r="J35" s="18"/>
-    </row>
-    <row r="36" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="13"/>
-      <c r="B36" s="14"/>
-      <c r="C36" s="34"/>
-      <c r="D36" s="16"/>
-      <c r="E36" s="15"/>
-      <c r="F36" s="15"/>
-      <c r="G36" s="17"/>
-      <c r="H36" s="17"/>
-      <c r="I36" s="17"/>
-      <c r="J36" s="18"/>
-    </row>
-    <row r="37" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="13"/>
-      <c r="B37" s="14"/>
-      <c r="C37" s="34"/>
-      <c r="D37" s="15"/>
-      <c r="E37" s="16"/>
-      <c r="F37" s="16"/>
-      <c r="G37" s="17"/>
-      <c r="H37" s="17"/>
-      <c r="I37" s="20"/>
-      <c r="J37" s="18"/>
-    </row>
-    <row r="38" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="13"/>
-      <c r="B38" s="14"/>
-      <c r="C38" s="34"/>
-      <c r="D38" s="15"/>
-      <c r="E38" s="16"/>
-      <c r="F38" s="16"/>
-      <c r="G38" s="17"/>
-      <c r="H38" s="17"/>
-      <c r="I38" s="17"/>
-      <c r="J38" s="18"/>
-    </row>
-    <row r="39" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="13"/>
-      <c r="B39" s="14"/>
-      <c r="C39" s="34"/>
-      <c r="D39" s="15"/>
-      <c r="E39" s="16"/>
-      <c r="F39" s="16"/>
-      <c r="G39" s="17"/>
-      <c r="H39" s="17"/>
-      <c r="I39" s="17"/>
-      <c r="J39" s="18"/>
-    </row>
-    <row r="40" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="13"/>
-      <c r="B40" s="14"/>
-      <c r="C40" s="34"/>
-      <c r="D40" s="15"/>
-      <c r="E40" s="16"/>
-      <c r="F40" s="16"/>
-      <c r="G40" s="17"/>
-      <c r="H40" s="21"/>
-      <c r="I40" s="17"/>
-      <c r="J40" s="18"/>
-    </row>
-    <row r="41" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="13"/>
-      <c r="B41" s="14"/>
-      <c r="C41" s="34"/>
-      <c r="D41" s="15"/>
-      <c r="E41" s="16"/>
-      <c r="F41" s="16"/>
-      <c r="G41" s="17"/>
-      <c r="H41" s="21"/>
-      <c r="I41" s="17"/>
-      <c r="J41" s="18"/>
-    </row>
-    <row r="42" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="13"/>
-      <c r="B42" s="22"/>
-      <c r="C42" s="37"/>
-      <c r="D42" s="23"/>
-      <c r="E42" s="23"/>
-      <c r="F42" s="23"/>
-      <c r="G42" s="21"/>
-      <c r="H42" s="21"/>
-      <c r="I42" s="17"/>
-      <c r="J42" s="16"/>
-    </row>
-    <row r="43" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="13"/>
-      <c r="B43" s="14"/>
-      <c r="C43" s="38"/>
-      <c r="D43" s="24"/>
-      <c r="E43" s="23"/>
-      <c r="F43" s="23"/>
-      <c r="G43" s="21"/>
-      <c r="H43" s="17"/>
-      <c r="I43" s="17"/>
-      <c r="J43" s="16"/>
-    </row>
-    <row r="44" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="13"/>
-      <c r="B44" s="14"/>
-      <c r="C44" s="34"/>
-      <c r="D44" s="15"/>
-      <c r="E44" s="23"/>
-      <c r="F44" s="23"/>
-      <c r="G44" s="17"/>
-      <c r="H44" s="17"/>
-      <c r="I44" s="17"/>
-      <c r="J44" s="16"/>
-    </row>
-    <row r="45" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="13"/>
-      <c r="B45" s="14"/>
-      <c r="C45" s="34"/>
-      <c r="D45" s="15"/>
-      <c r="E45" s="16"/>
-      <c r="F45" s="16"/>
-      <c r="G45" s="17"/>
-      <c r="H45" s="17"/>
-      <c r="I45" s="17"/>
-      <c r="J45" s="16"/>
-    </row>
-    <row r="46" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="13"/>
-      <c r="B46" s="14"/>
-      <c r="C46" s="34"/>
-      <c r="D46" s="16"/>
-      <c r="E46" s="16"/>
-      <c r="F46" s="16"/>
-      <c r="G46" s="17"/>
-      <c r="H46" s="17"/>
-      <c r="I46" s="17"/>
-      <c r="J46" s="16"/>
-    </row>
-    <row r="47" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="13"/>
-      <c r="B47" s="14"/>
-      <c r="C47" s="34"/>
-      <c r="D47" s="16"/>
-      <c r="E47" s="16"/>
-      <c r="F47" s="16"/>
-      <c r="G47" s="21"/>
-      <c r="H47" s="17"/>
-      <c r="I47" s="17"/>
-      <c r="J47" s="16"/>
-    </row>
-    <row r="48" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="13"/>
-      <c r="B48" s="16"/>
-      <c r="C48" s="34"/>
-      <c r="D48" s="16"/>
-      <c r="E48" s="16"/>
-      <c r="F48" s="16"/>
-      <c r="G48" s="21"/>
-      <c r="H48" s="17"/>
-      <c r="I48" s="17"/>
-      <c r="J48" s="16"/>
-    </row>
-    <row r="49" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="13"/>
-      <c r="B49" s="14"/>
-      <c r="C49" s="34"/>
-      <c r="D49" s="16"/>
-      <c r="E49" s="16"/>
-      <c r="F49" s="16"/>
-      <c r="G49" s="21"/>
-      <c r="H49" s="17"/>
-      <c r="I49" s="17"/>
-      <c r="J49" s="16"/>
-    </row>
-    <row r="50" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="13"/>
-      <c r="B50" s="14"/>
-      <c r="C50" s="39"/>
-      <c r="D50" s="15"/>
-      <c r="E50" s="16"/>
-      <c r="F50" s="16"/>
-      <c r="G50" s="17"/>
-      <c r="H50" s="17"/>
-      <c r="I50" s="17"/>
-      <c r="J50" s="16"/>
-    </row>
-    <row r="51" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="13"/>
-      <c r="B51" s="14"/>
-      <c r="C51" s="39"/>
-      <c r="D51" s="15"/>
-      <c r="E51" s="16"/>
-      <c r="F51" s="16"/>
-      <c r="G51" s="17"/>
-      <c r="H51" s="17"/>
-      <c r="I51" s="17"/>
-      <c r="J51" s="16"/>
-    </row>
-    <row r="52" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="13"/>
-      <c r="B52" s="14"/>
-      <c r="C52" s="34"/>
-      <c r="D52" s="15"/>
-      <c r="E52" s="16"/>
-      <c r="F52" s="16"/>
-      <c r="G52" s="17"/>
-      <c r="H52" s="17"/>
-      <c r="I52" s="17"/>
-      <c r="J52" s="16"/>
-    </row>
-    <row r="53" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="13"/>
-      <c r="B53" s="14"/>
-      <c r="C53" s="34"/>
-      <c r="D53" s="16"/>
-      <c r="E53" s="16"/>
-      <c r="F53" s="16"/>
-      <c r="G53" s="17"/>
-      <c r="H53" s="20"/>
-      <c r="I53" s="17"/>
-      <c r="J53" s="16"/>
-    </row>
-    <row r="54" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="13"/>
-      <c r="B54" s="25"/>
-      <c r="C54" s="40"/>
-      <c r="D54" s="26"/>
-      <c r="E54" s="27"/>
-      <c r="F54" s="27"/>
-      <c r="G54" s="28"/>
-      <c r="H54" s="28"/>
-      <c r="I54" s="28"/>
-      <c r="J54" s="16"/>
-    </row>
-    <row r="55" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="29"/>
-      <c r="B55" s="30"/>
-      <c r="C55" s="41"/>
-      <c r="D55" s="32"/>
-      <c r="E55" s="30"/>
-      <c r="F55" s="30"/>
-      <c r="G55" s="33"/>
-      <c r="H55" s="33"/>
-      <c r="I55" s="33"/>
-      <c r="J55" s="16"/>
-    </row>
-    <row r="56" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="29"/>
-      <c r="B56" s="31"/>
-      <c r="C56" s="41"/>
-      <c r="D56" s="32"/>
-      <c r="E56" s="30"/>
-      <c r="F56" s="30"/>
-      <c r="G56" s="33"/>
-      <c r="H56" s="33"/>
-      <c r="I56" s="33"/>
-      <c r="J56" s="16"/>
-    </row>
-    <row r="57" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="29"/>
-      <c r="B57" s="31"/>
-      <c r="C57" s="41"/>
-      <c r="D57" s="32"/>
-      <c r="E57" s="30"/>
-      <c r="F57" s="30"/>
-      <c r="G57" s="33"/>
-      <c r="H57" s="33"/>
-      <c r="I57" s="33"/>
-      <c r="J57" s="16"/>
-    </row>
-    <row r="58" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="29"/>
-      <c r="B58" s="31"/>
-      <c r="C58" s="41"/>
-      <c r="D58" s="30"/>
-      <c r="E58" s="32"/>
-      <c r="F58" s="32"/>
-      <c r="G58" s="33"/>
-      <c r="H58" s="33"/>
-      <c r="I58" s="33"/>
-      <c r="J58" s="16"/>
-    </row>
-    <row r="59" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="11"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="5"/>
+    </row>
+    <row r="33" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="11"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
+      <c r="I33" s="5"/>
+    </row>
+    <row r="34" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="11"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="5"/>
+      <c r="H34" s="5"/>
+      <c r="I34" s="5"/>
+    </row>
+    <row r="35" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="11"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="5"/>
+      <c r="H35" s="5"/>
+      <c r="I35" s="5"/>
+    </row>
+    <row r="36" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="11"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="5"/>
+      <c r="H36" s="5"/>
+      <c r="I36" s="5"/>
+    </row>
+    <row r="37" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="11"/>
+      <c r="B37" s="3"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="5"/>
+      <c r="H37" s="5"/>
+      <c r="I37" s="5"/>
+    </row>
+    <row r="38" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="11"/>
+      <c r="B38" s="3"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="5"/>
+      <c r="H38" s="5"/>
+      <c r="I38" s="5"/>
+    </row>
+    <row r="39" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="11"/>
+      <c r="B39" s="3"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="5"/>
+      <c r="H39" s="5"/>
+      <c r="I39" s="5"/>
+    </row>
+    <row r="40" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="11"/>
+      <c r="B40" s="3"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="5"/>
+      <c r="H40" s="5"/>
+      <c r="I40" s="5"/>
+    </row>
+    <row r="41" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="11"/>
+      <c r="B41" s="3"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="5"/>
+      <c r="H41" s="5"/>
+      <c r="I41" s="5"/>
+    </row>
+    <row r="42" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="11"/>
+      <c r="B42" s="3"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="5"/>
+      <c r="H42" s="5"/>
+      <c r="I42" s="5"/>
+    </row>
+    <row r="43" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="11"/>
+      <c r="B43" s="3"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3"/>
+      <c r="G43" s="5"/>
+      <c r="H43" s="5"/>
+      <c r="I43" s="5"/>
+    </row>
+    <row r="44" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="11"/>
+      <c r="B44" s="3"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3"/>
+      <c r="G44" s="5"/>
+      <c r="H44" s="5"/>
+      <c r="I44" s="5"/>
+    </row>
+    <row r="45" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="11"/>
+      <c r="B45" s="3"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3"/>
+      <c r="G45" s="5"/>
+      <c r="H45" s="5"/>
+      <c r="I45" s="5"/>
+    </row>
+    <row r="46" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="11"/>
+      <c r="B46" s="3"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
+      <c r="G46" s="5"/>
+      <c r="H46" s="5"/>
+      <c r="I46" s="5"/>
+    </row>
+    <row r="47" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="11"/>
+      <c r="B47" s="3"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
+      <c r="G47" s="5"/>
+      <c r="H47" s="5"/>
+      <c r="I47" s="5"/>
+    </row>
+    <row r="48" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="11"/>
+      <c r="B48" s="3"/>
+      <c r="C48" s="5"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3"/>
+      <c r="F48" s="3"/>
+      <c r="G48" s="5"/>
+      <c r="H48" s="5"/>
+      <c r="I48" s="5"/>
+    </row>
+    <row r="49" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="11"/>
+      <c r="B49" s="3"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="3"/>
+      <c r="F49" s="3"/>
+      <c r="G49" s="5"/>
+      <c r="H49" s="5"/>
+      <c r="I49" s="5"/>
+    </row>
+    <row r="50" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="11"/>
+      <c r="B50" s="3"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="3"/>
+      <c r="E50" s="3"/>
+      <c r="F50" s="3"/>
+      <c r="G50" s="5"/>
+      <c r="H50" s="5"/>
+      <c r="I50" s="5"/>
+    </row>
+    <row r="51" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="11"/>
+      <c r="B51" s="3"/>
+      <c r="C51" s="5"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="3"/>
+      <c r="F51" s="3"/>
+      <c r="G51" s="5"/>
+      <c r="H51" s="5"/>
+      <c r="I51" s="5"/>
+    </row>
+    <row r="52" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="11"/>
+      <c r="B52" s="3"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3"/>
+      <c r="F52" s="3"/>
+      <c r="G52" s="5"/>
+      <c r="H52" s="5"/>
+      <c r="I52" s="5"/>
+    </row>
+    <row r="53" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="11"/>
+      <c r="B53" s="3"/>
+      <c r="C53" s="5"/>
+      <c r="D53" s="3"/>
+      <c r="E53" s="3"/>
+      <c r="F53" s="3"/>
+      <c r="G53" s="5"/>
+      <c r="H53" s="5"/>
+      <c r="I53" s="5"/>
+    </row>
+    <row r="54" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="11"/>
+      <c r="B54" s="3"/>
+      <c r="C54" s="5"/>
+      <c r="D54" s="3"/>
+      <c r="E54" s="3"/>
+      <c r="F54" s="3"/>
+      <c r="G54" s="5"/>
+      <c r="H54" s="5"/>
+      <c r="I54" s="5"/>
+    </row>
+    <row r="55" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="11"/>
+      <c r="B55" s="3"/>
+      <c r="C55" s="5"/>
+      <c r="D55" s="3"/>
+      <c r="E55" s="3"/>
+      <c r="F55" s="3"/>
+      <c r="G55" s="5"/>
+      <c r="H55" s="5"/>
+      <c r="I55" s="5"/>
+    </row>
+    <row r="56" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="11"/>
+      <c r="B56" s="3"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="3"/>
+      <c r="E56" s="3"/>
+      <c r="F56" s="3"/>
+      <c r="G56" s="5"/>
+      <c r="H56" s="5"/>
+      <c r="I56" s="5"/>
+    </row>
+    <row r="57" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="11"/>
+      <c r="B57" s="3"/>
+      <c r="C57" s="5"/>
+      <c r="D57" s="3"/>
+      <c r="E57" s="3"/>
+      <c r="F57" s="3"/>
+      <c r="G57" s="5"/>
+      <c r="H57" s="5"/>
+      <c r="I57" s="5"/>
+    </row>
+    <row r="58" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="11"/>
+      <c r="B58" s="3"/>
+      <c r="C58" s="5"/>
+      <c r="D58" s="3"/>
+      <c r="E58" s="3"/>
+      <c r="F58" s="3"/>
+      <c r="G58" s="5"/>
+      <c r="H58" s="5"/>
+      <c r="I58" s="5"/>
+    </row>
+    <row r="59" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="11"/>
       <c r="B59" s="3"/>
       <c r="C59" s="5"/>
@@ -1509,7 +1411,7 @@
       <c r="H59" s="5"/>
       <c r="I59" s="5"/>
     </row>
-    <row r="60" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="11"/>
       <c r="B60" s="3"/>
       <c r="C60" s="5"/>
@@ -1520,7 +1422,7 @@
       <c r="H60" s="5"/>
       <c r="I60" s="5"/>
     </row>
-    <row r="61" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="11"/>
       <c r="B61" s="3"/>
       <c r="C61" s="5"/>
@@ -1531,8 +1433,7 @@
       <c r="H61" s="5"/>
       <c r="I61" s="5"/>
     </row>
-    <row r="62" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="11"/>
+    <row r="62" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B62" s="3"/>
       <c r="C62" s="5"/>
       <c r="D62" s="3"/>
@@ -1542,8 +1443,7 @@
       <c r="H62" s="5"/>
       <c r="I62" s="5"/>
     </row>
-    <row r="63" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="11"/>
+    <row r="63" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B63" s="3"/>
       <c r="C63" s="5"/>
       <c r="D63" s="3"/>
@@ -1553,8 +1453,7 @@
       <c r="H63" s="5"/>
       <c r="I63" s="5"/>
     </row>
-    <row r="64" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="11"/>
+    <row r="64" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" s="3"/>
       <c r="C64" s="5"/>
       <c r="D64" s="3"/>
@@ -1564,8 +1463,7 @@
       <c r="H64" s="5"/>
       <c r="I64" s="5"/>
     </row>
-    <row r="65" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="11"/>
+    <row r="65" spans="2:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B65" s="3"/>
       <c r="C65" s="5"/>
       <c r="D65" s="3"/>
@@ -1575,8 +1473,7 @@
       <c r="H65" s="5"/>
       <c r="I65" s="5"/>
     </row>
-    <row r="66" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="11"/>
+    <row r="66" spans="2:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B66" s="3"/>
       <c r="C66" s="5"/>
       <c r="D66" s="3"/>
@@ -1586,8 +1483,7 @@
       <c r="H66" s="5"/>
       <c r="I66" s="5"/>
     </row>
-    <row r="67" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="11"/>
+    <row r="67" spans="2:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B67" s="3"/>
       <c r="C67" s="5"/>
       <c r="D67" s="3"/>
@@ -1597,8 +1493,7 @@
       <c r="H67" s="5"/>
       <c r="I67" s="5"/>
     </row>
-    <row r="68" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="11"/>
+    <row r="68" spans="2:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B68" s="3"/>
       <c r="C68" s="5"/>
       <c r="D68" s="3"/>
@@ -1608,8 +1503,7 @@
       <c r="H68" s="5"/>
       <c r="I68" s="5"/>
     </row>
-    <row r="69" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="11"/>
+    <row r="69" spans="2:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B69" s="3"/>
       <c r="C69" s="5"/>
       <c r="D69" s="3"/>
@@ -1619,8 +1513,7 @@
       <c r="H69" s="5"/>
       <c r="I69" s="5"/>
     </row>
-    <row r="70" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="11"/>
+    <row r="70" spans="2:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B70" s="3"/>
       <c r="C70" s="5"/>
       <c r="D70" s="3"/>
@@ -1630,8 +1523,7 @@
       <c r="H70" s="5"/>
       <c r="I70" s="5"/>
     </row>
-    <row r="71" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="11"/>
+    <row r="71" spans="2:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B71" s="3"/>
       <c r="C71" s="5"/>
       <c r="D71" s="3"/>
@@ -1641,8 +1533,7 @@
       <c r="H71" s="5"/>
       <c r="I71" s="5"/>
     </row>
-    <row r="72" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="11"/>
+    <row r="72" spans="2:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B72" s="3"/>
       <c r="C72" s="5"/>
       <c r="D72" s="3"/>
@@ -1652,8 +1543,7 @@
       <c r="H72" s="5"/>
       <c r="I72" s="5"/>
     </row>
-    <row r="73" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="11"/>
+    <row r="73" spans="2:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B73" s="3"/>
       <c r="C73" s="5"/>
       <c r="D73" s="3"/>
@@ -1663,8 +1553,7 @@
       <c r="H73" s="5"/>
       <c r="I73" s="5"/>
     </row>
-    <row r="74" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="11"/>
+    <row r="74" spans="2:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B74" s="3"/>
       <c r="C74" s="5"/>
       <c r="D74" s="3"/>
@@ -1674,8 +1563,7 @@
       <c r="H74" s="5"/>
       <c r="I74" s="5"/>
     </row>
-    <row r="75" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="11"/>
+    <row r="75" spans="2:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B75" s="3"/>
       <c r="C75" s="5"/>
       <c r="D75" s="3"/>
@@ -1685,8 +1573,7 @@
       <c r="H75" s="5"/>
       <c r="I75" s="5"/>
     </row>
-    <row r="76" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="11"/>
+    <row r="76" spans="2:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B76" s="3"/>
       <c r="C76" s="5"/>
       <c r="D76" s="3"/>
@@ -1696,8 +1583,7 @@
       <c r="H76" s="5"/>
       <c r="I76" s="5"/>
     </row>
-    <row r="77" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="11"/>
+    <row r="77" spans="2:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B77" s="3"/>
       <c r="C77" s="5"/>
       <c r="D77" s="3"/>
@@ -1707,8 +1593,7 @@
       <c r="H77" s="5"/>
       <c r="I77" s="5"/>
     </row>
-    <row r="78" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="11"/>
+    <row r="78" spans="2:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B78" s="3"/>
       <c r="C78" s="5"/>
       <c r="D78" s="3"/>
@@ -1718,8 +1603,7 @@
       <c r="H78" s="5"/>
       <c r="I78" s="5"/>
     </row>
-    <row r="79" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="11"/>
+    <row r="79" spans="2:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B79" s="3"/>
       <c r="C79" s="5"/>
       <c r="D79" s="3"/>
@@ -1729,8 +1613,7 @@
       <c r="H79" s="5"/>
       <c r="I79" s="5"/>
     </row>
-    <row r="80" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="11"/>
+    <row r="80" spans="2:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B80" s="3"/>
       <c r="C80" s="5"/>
       <c r="D80" s="3"/>
@@ -1740,8 +1623,7 @@
       <c r="H80" s="5"/>
       <c r="I80" s="5"/>
     </row>
-    <row r="81" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="11"/>
+    <row r="81" spans="2:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B81" s="3"/>
       <c r="C81" s="5"/>
       <c r="D81" s="3"/>
@@ -1751,8 +1633,7 @@
       <c r="H81" s="5"/>
       <c r="I81" s="5"/>
     </row>
-    <row r="82" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="11"/>
+    <row r="82" spans="2:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B82" s="3"/>
       <c r="C82" s="5"/>
       <c r="D82" s="3"/>
@@ -1762,8 +1643,7 @@
       <c r="H82" s="5"/>
       <c r="I82" s="5"/>
     </row>
-    <row r="83" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="11"/>
+    <row r="83" spans="2:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B83" s="3"/>
       <c r="C83" s="5"/>
       <c r="D83" s="3"/>
@@ -1773,8 +1653,7 @@
       <c r="H83" s="5"/>
       <c r="I83" s="5"/>
     </row>
-    <row r="84" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="11"/>
+    <row r="84" spans="2:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B84" s="3"/>
       <c r="C84" s="5"/>
       <c r="D84" s="3"/>
@@ -1784,8 +1663,7 @@
       <c r="H84" s="5"/>
       <c r="I84" s="5"/>
     </row>
-    <row r="85" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="11"/>
+    <row r="85" spans="2:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B85" s="3"/>
       <c r="C85" s="5"/>
       <c r="D85" s="3"/>
@@ -1795,8 +1673,7 @@
       <c r="H85" s="5"/>
       <c r="I85" s="5"/>
     </row>
-    <row r="86" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="11"/>
+    <row r="86" spans="2:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B86" s="3"/>
       <c r="C86" s="5"/>
       <c r="D86" s="3"/>
@@ -1806,8 +1683,7 @@
       <c r="H86" s="5"/>
       <c r="I86" s="5"/>
     </row>
-    <row r="87" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="11"/>
+    <row r="87" spans="2:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B87" s="3"/>
       <c r="C87" s="5"/>
       <c r="D87" s="3"/>
@@ -1817,8 +1693,7 @@
       <c r="H87" s="5"/>
       <c r="I87" s="5"/>
     </row>
-    <row r="88" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="11"/>
+    <row r="88" spans="2:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B88" s="3"/>
       <c r="C88" s="5"/>
       <c r="D88" s="3"/>
@@ -1828,7 +1703,7 @@
       <c r="H88" s="5"/>
       <c r="I88" s="5"/>
     </row>
-    <row r="89" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B89" s="3"/>
       <c r="C89" s="5"/>
       <c r="D89" s="3"/>
@@ -1838,7 +1713,7 @@
       <c r="H89" s="5"/>
       <c r="I89" s="5"/>
     </row>
-    <row r="90" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B90" s="3"/>
       <c r="C90" s="5"/>
       <c r="D90" s="3"/>
@@ -1848,7 +1723,7 @@
       <c r="H90" s="5"/>
       <c r="I90" s="5"/>
     </row>
-    <row r="91" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B91" s="3"/>
       <c r="C91" s="5"/>
       <c r="D91" s="3"/>
@@ -1858,7 +1733,7 @@
       <c r="H91" s="5"/>
       <c r="I91" s="5"/>
     </row>
-    <row r="92" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B92" s="3"/>
       <c r="C92" s="5"/>
       <c r="D92" s="3"/>
@@ -1868,7 +1743,7 @@
       <c r="H92" s="5"/>
       <c r="I92" s="5"/>
     </row>
-    <row r="93" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B93" s="3"/>
       <c r="C93" s="5"/>
       <c r="D93" s="3"/>
@@ -1878,7 +1753,7 @@
       <c r="H93" s="5"/>
       <c r="I93" s="5"/>
     </row>
-    <row r="94" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B94" s="3"/>
       <c r="C94" s="5"/>
       <c r="D94" s="3"/>
@@ -1888,7 +1763,7 @@
       <c r="H94" s="5"/>
       <c r="I94" s="5"/>
     </row>
-    <row r="95" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B95" s="3"/>
       <c r="C95" s="5"/>
       <c r="D95" s="3"/>
@@ -1898,7 +1773,7 @@
       <c r="H95" s="5"/>
       <c r="I95" s="5"/>
     </row>
-    <row r="96" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B96" s="3"/>
       <c r="C96" s="5"/>
       <c r="D96" s="3"/>
@@ -10057,276 +9932,6 @@
       <c r="G911" s="5"/>
       <c r="H911" s="5"/>
       <c r="I911" s="5"/>
-    </row>
-    <row r="912" spans="2:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B912" s="3"/>
-      <c r="C912" s="5"/>
-      <c r="D912" s="3"/>
-      <c r="E912" s="3"/>
-      <c r="F912" s="3"/>
-      <c r="G912" s="5"/>
-      <c r="H912" s="5"/>
-      <c r="I912" s="5"/>
-    </row>
-    <row r="913" spans="2:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B913" s="3"/>
-      <c r="C913" s="5"/>
-      <c r="D913" s="3"/>
-      <c r="E913" s="3"/>
-      <c r="F913" s="3"/>
-      <c r="G913" s="5"/>
-      <c r="H913" s="5"/>
-      <c r="I913" s="5"/>
-    </row>
-    <row r="914" spans="2:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B914" s="3"/>
-      <c r="C914" s="5"/>
-      <c r="D914" s="3"/>
-      <c r="E914" s="3"/>
-      <c r="F914" s="3"/>
-      <c r="G914" s="5"/>
-      <c r="H914" s="5"/>
-      <c r="I914" s="5"/>
-    </row>
-    <row r="915" spans="2:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B915" s="3"/>
-      <c r="C915" s="5"/>
-      <c r="D915" s="3"/>
-      <c r="E915" s="3"/>
-      <c r="F915" s="3"/>
-      <c r="G915" s="5"/>
-      <c r="H915" s="5"/>
-      <c r="I915" s="5"/>
-    </row>
-    <row r="916" spans="2:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B916" s="3"/>
-      <c r="C916" s="5"/>
-      <c r="D916" s="3"/>
-      <c r="E916" s="3"/>
-      <c r="F916" s="3"/>
-      <c r="G916" s="5"/>
-      <c r="H916" s="5"/>
-      <c r="I916" s="5"/>
-    </row>
-    <row r="917" spans="2:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B917" s="3"/>
-      <c r="C917" s="5"/>
-      <c r="D917" s="3"/>
-      <c r="E917" s="3"/>
-      <c r="F917" s="3"/>
-      <c r="G917" s="5"/>
-      <c r="H917" s="5"/>
-      <c r="I917" s="5"/>
-    </row>
-    <row r="918" spans="2:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B918" s="3"/>
-      <c r="C918" s="5"/>
-      <c r="D918" s="3"/>
-      <c r="E918" s="3"/>
-      <c r="F918" s="3"/>
-      <c r="G918" s="5"/>
-      <c r="H918" s="5"/>
-      <c r="I918" s="5"/>
-    </row>
-    <row r="919" spans="2:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B919" s="3"/>
-      <c r="C919" s="5"/>
-      <c r="D919" s="3"/>
-      <c r="E919" s="3"/>
-      <c r="F919" s="3"/>
-      <c r="G919" s="5"/>
-      <c r="H919" s="5"/>
-      <c r="I919" s="5"/>
-    </row>
-    <row r="920" spans="2:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B920" s="3"/>
-      <c r="C920" s="5"/>
-      <c r="D920" s="3"/>
-      <c r="E920" s="3"/>
-      <c r="F920" s="3"/>
-      <c r="G920" s="5"/>
-      <c r="H920" s="5"/>
-      <c r="I920" s="5"/>
-    </row>
-    <row r="921" spans="2:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B921" s="3"/>
-      <c r="C921" s="5"/>
-      <c r="D921" s="3"/>
-      <c r="E921" s="3"/>
-      <c r="F921" s="3"/>
-      <c r="G921" s="5"/>
-      <c r="H921" s="5"/>
-      <c r="I921" s="5"/>
-    </row>
-    <row r="922" spans="2:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B922" s="3"/>
-      <c r="C922" s="5"/>
-      <c r="D922" s="3"/>
-      <c r="E922" s="3"/>
-      <c r="F922" s="3"/>
-      <c r="G922" s="5"/>
-      <c r="H922" s="5"/>
-      <c r="I922" s="5"/>
-    </row>
-    <row r="923" spans="2:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B923" s="3"/>
-      <c r="C923" s="5"/>
-      <c r="D923" s="3"/>
-      <c r="E923" s="3"/>
-      <c r="F923" s="3"/>
-      <c r="G923" s="5"/>
-      <c r="H923" s="5"/>
-      <c r="I923" s="5"/>
-    </row>
-    <row r="924" spans="2:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B924" s="3"/>
-      <c r="C924" s="5"/>
-      <c r="D924" s="3"/>
-      <c r="E924" s="3"/>
-      <c r="F924" s="3"/>
-      <c r="G924" s="5"/>
-      <c r="H924" s="5"/>
-      <c r="I924" s="5"/>
-    </row>
-    <row r="925" spans="2:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B925" s="3"/>
-      <c r="C925" s="5"/>
-      <c r="D925" s="3"/>
-      <c r="E925" s="3"/>
-      <c r="F925" s="3"/>
-      <c r="G925" s="5"/>
-      <c r="H925" s="5"/>
-      <c r="I925" s="5"/>
-    </row>
-    <row r="926" spans="2:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B926" s="3"/>
-      <c r="C926" s="5"/>
-      <c r="D926" s="3"/>
-      <c r="E926" s="3"/>
-      <c r="F926" s="3"/>
-      <c r="G926" s="5"/>
-      <c r="H926" s="5"/>
-      <c r="I926" s="5"/>
-    </row>
-    <row r="927" spans="2:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B927" s="3"/>
-      <c r="C927" s="5"/>
-      <c r="D927" s="3"/>
-      <c r="E927" s="3"/>
-      <c r="F927" s="3"/>
-      <c r="G927" s="5"/>
-      <c r="H927" s="5"/>
-      <c r="I927" s="5"/>
-    </row>
-    <row r="928" spans="2:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B928" s="3"/>
-      <c r="C928" s="5"/>
-      <c r="D928" s="3"/>
-      <c r="E928" s="3"/>
-      <c r="F928" s="3"/>
-      <c r="G928" s="5"/>
-      <c r="H928" s="5"/>
-      <c r="I928" s="5"/>
-    </row>
-    <row r="929" spans="2:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B929" s="3"/>
-      <c r="C929" s="5"/>
-      <c r="D929" s="3"/>
-      <c r="E929" s="3"/>
-      <c r="F929" s="3"/>
-      <c r="G929" s="5"/>
-      <c r="H929" s="5"/>
-      <c r="I929" s="5"/>
-    </row>
-    <row r="930" spans="2:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B930" s="3"/>
-      <c r="C930" s="5"/>
-      <c r="D930" s="3"/>
-      <c r="E930" s="3"/>
-      <c r="F930" s="3"/>
-      <c r="G930" s="5"/>
-      <c r="H930" s="5"/>
-      <c r="I930" s="5"/>
-    </row>
-    <row r="931" spans="2:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B931" s="3"/>
-      <c r="C931" s="5"/>
-      <c r="D931" s="3"/>
-      <c r="E931" s="3"/>
-      <c r="F931" s="3"/>
-      <c r="G931" s="5"/>
-      <c r="H931" s="5"/>
-      <c r="I931" s="5"/>
-    </row>
-    <row r="932" spans="2:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B932" s="3"/>
-      <c r="C932" s="5"/>
-      <c r="D932" s="3"/>
-      <c r="E932" s="3"/>
-      <c r="F932" s="3"/>
-      <c r="G932" s="5"/>
-      <c r="H932" s="5"/>
-      <c r="I932" s="5"/>
-    </row>
-    <row r="933" spans="2:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B933" s="3"/>
-      <c r="C933" s="5"/>
-      <c r="D933" s="3"/>
-      <c r="E933" s="3"/>
-      <c r="F933" s="3"/>
-      <c r="G933" s="5"/>
-      <c r="H933" s="5"/>
-      <c r="I933" s="5"/>
-    </row>
-    <row r="934" spans="2:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B934" s="3"/>
-      <c r="C934" s="5"/>
-      <c r="D934" s="3"/>
-      <c r="E934" s="3"/>
-      <c r="F934" s="3"/>
-      <c r="G934" s="5"/>
-      <c r="H934" s="5"/>
-      <c r="I934" s="5"/>
-    </row>
-    <row r="935" spans="2:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B935" s="3"/>
-      <c r="C935" s="5"/>
-      <c r="D935" s="3"/>
-      <c r="E935" s="3"/>
-      <c r="F935" s="3"/>
-      <c r="G935" s="5"/>
-      <c r="H935" s="5"/>
-      <c r="I935" s="5"/>
-    </row>
-    <row r="936" spans="2:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B936" s="3"/>
-      <c r="C936" s="5"/>
-      <c r="D936" s="3"/>
-      <c r="E936" s="3"/>
-      <c r="F936" s="3"/>
-      <c r="G936" s="5"/>
-      <c r="H936" s="5"/>
-      <c r="I936" s="5"/>
-    </row>
-    <row r="937" spans="2:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B937" s="3"/>
-      <c r="C937" s="5"/>
-      <c r="D937" s="3"/>
-      <c r="E937" s="3"/>
-      <c r="F937" s="3"/>
-      <c r="G937" s="5"/>
-      <c r="H937" s="5"/>
-      <c r="I937" s="5"/>
-    </row>
-    <row r="938" spans="2:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B938" s="3"/>
-      <c r="C938" s="5"/>
-      <c r="D938" s="3"/>
-      <c r="E938" s="3"/>
-      <c r="F938" s="3"/>
-      <c r="G938" s="5"/>
-      <c r="H938" s="5"/>
-      <c r="I938" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="11">

</xml_diff>